<commit_message>
updating indicators from most meas
</commit_message>
<xml_diff>
--- a/input/meas/RAMSAR/ramsar.xlsx
+++ b/input/meas/RAMSAR/ramsar.xlsx
@@ -78,7 +78,9 @@
 47% of Contracting Parties have included wetland issues within National Policies or measures on agriculture. (National Reports to COP12). </t>
   </si>
   <si>
-    <t>% of Parties that have made assessment of ecosystem services of Ramsar Sites. (Data source: National Reports); % of Parties that have included wetland issues within national strategies and planning processes such as water resource management and water efficiency plans. (Data source: National Reports); % of Parties that have included wetland issues within National Policies or measures on agriculture. (Data source: National Reports).</t>
+    <t>% of Parties that have made assessment of ecosystem services of Ramsar Sites. (Data source: National Reports)
+% of Parties that have included wetland issues within national strategies and planning processes such as water resource management and water efficiency plans. (Data source: National Reports)
+% of Parties that have included wetland issues within National Policies or measures on agriculture. (Data source: National Reports).</t>
   </si>
   <si>
     <t>RAMSAR_SG1_T2</t>

</xml_diff>